<commit_message>
week 3 data spr 22
</commit_message>
<xml_diff>
--- a/data/wookieMistakesPlayerData.xlsx
+++ b/data/wookieMistakesPlayerData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d53cb9c05b082722/Documents/apa-rankings/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://onedrive.homedepot.com/personal/scott_r_berry_homedepot_com/Documents/apa-rankings/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="11_F25DC773A252ABDACC1048B9E9184DC65ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A8D2092-997A-4DB6-B63E-407E51957032}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="11_F25DC773A252ABDACC1048B9E9184DC65ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C857D7A0-2E33-6B49-8A8E-26703E935BB3}"/>
   <bookViews>
-    <workbookView xWindow="21675" yWindow="2925" windowWidth="15150" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21680" yWindow="2920" windowWidth="15160" windowHeight="11380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -381,18 +381,18 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -406,7 +406,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -420,7 +420,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -434,7 +434,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -448,7 +448,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -459,10 +459,10 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -470,13 +470,13 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -487,10 +487,10 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -498,13 +498,13 @@
         <v>3</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -512,10 +512,10 @@
         <v>6</v>
       </c>
       <c r="C9">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D9">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>

</xml_diff>